<commit_message>
swap out cases in test to be consistent
</commit_message>
<xml_diff>
--- a/data/ground_truth_test1.xlsx
+++ b/data/ground_truth_test1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ScottFerrier\Desktop\LLM-Compl-Sum\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ScottFerrier\Desktop\LLM-Complaint-Summary-Test\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45C44FAB-72FE-4820-9B87-330F0CF822A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3CAAE05-37FC-434B-9BF8-BDAF2649EEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12720" yWindow="0" windowWidth="12960" windowHeight="13760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="142">
   <si>
     <t>case_id</t>
   </si>
@@ -115,21 +115,6 @@
     <t>Section 15 of the Securities Act</t>
   </si>
   <si>
-    <t>cand_22_cv_00105</t>
-  </si>
-  <si>
-    <t>Martin Dugan, Leon Yu, and Max Wisdom Technology Limited</t>
-  </si>
-  <si>
-    <t>Talis Biomedical Corporation, Brian Coe, J. Roger Moody, Jr., Felix Baker, Raymond Cheong, Melissa Gilliam, Rustem F. Ismagilov, Kimberly J. Popovits, Matthew L. Posard, and Randal Scott</t>
-  </si>
-  <si>
-    <t>TLIS</t>
-  </si>
-  <si>
-    <t>Section 10(b) of the Exchange Act</t>
-  </si>
-  <si>
     <t>cand_22_cv_02094</t>
   </si>
   <si>
@@ -187,21 +172,6 @@
     <t>VICR</t>
   </si>
   <si>
-    <t>cand_3_21-cv-09767</t>
-  </si>
-  <si>
-    <t>Vinod Sodha and Amee Sodha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Robinhood Markets, Inc., Vladimir Tenev, Jason Warnick, Jan Hammer, Paula Loop, Jonathan Rubenstein, Scott Sandell, Robert Zoellick, Goldman Sachs &amp; Co. LLC, J.P. Morgan Securities LLC, Barclays Capital Inc., Citigroup Global Markets Inc., Wells Fargo Securities, LLC, Mizuho Securities USA LLC, JMP Securities LLC, KeyBanc Capital Markets Inc., Piper Sandler &amp; Co. , Rosenblatt Securities Inc. , BTIG, LLC, Santander Investment Securities Inc., Academy Securities, Inc., Loop Capital Markets LLC, Samuel A. Ramirez &amp; Company, Inc., and Siebert Williams Shank &amp; Co. LLC </t>
-  </si>
-  <si>
-    <t>HOOD</t>
-  </si>
-  <si>
-    <t>Section 12(a) of the Securities Act</t>
-  </si>
-  <si>
     <t>cand_3_22-cv-00956</t>
   </si>
   <si>
@@ -248,78 +218,6 @@
   </si>
   <si>
     <t>IBRX</t>
-  </si>
-  <si>
-    <t>ctd-3_24-cv-01727</t>
-  </si>
-  <si>
-    <t>United States Securities and Exchange Commission</t>
-  </si>
-  <si>
-    <t>The Lovesac Company, Donna Dellomo, and Yoon Um</t>
-  </si>
-  <si>
-    <t>LOVE</t>
-  </si>
-  <si>
-    <t>Securities Act Sections 17(a)(1) and (3)</t>
-  </si>
-  <si>
-    <t>Securities Act Section 17(a)(3)</t>
-  </si>
-  <si>
-    <t>Exchange Act Section 10(b) and Rules 10b-5(a) and (c)</t>
-  </si>
-  <si>
-    <t>Exchange Act Section 10(b) and Rule 10b-5(b)</t>
-  </si>
-  <si>
-    <t>Exchange Act Section 13(b)(5)</t>
-  </si>
-  <si>
-    <t>Exchange Act Rule 13b2-1</t>
-  </si>
-  <si>
-    <t>Section Exchange Act Rule 13b2-2</t>
-  </si>
-  <si>
-    <t>Exchange Act Section 13(a) and Rules 12b-20, 13a-1, 13a-11, and 13a-13</t>
-  </si>
-  <si>
-    <t>Aiding and abetting violations of Exchange Act Section 13(a) and Rules 12b-20, 13a-1, 13a-11, and 13a-13</t>
-  </si>
-  <si>
-    <t>Exchange Act Rule 13a-14</t>
-  </si>
-  <si>
-    <t>Exchange Act Section 13(b)(2)(B)</t>
-  </si>
-  <si>
-    <t>dcd-1_23-cv-01599</t>
-  </si>
-  <si>
-    <t>Securities and Exchange Commission</t>
-  </si>
-  <si>
-    <t>Binance Holdings Limited, BAM Trading Services Inc., BAM Management US Holdings Inc., and Changpeng Zhao</t>
-  </si>
-  <si>
-    <t>Sections 5(a) and 5(c) of the Securities Act</t>
-  </si>
-  <si>
-    <t>Exchange Act Section 5</t>
-  </si>
-  <si>
-    <t>Exchange Act Section 15(a)</t>
-  </si>
-  <si>
-    <t>Exchange Act Section 17A(b)</t>
-  </si>
-  <si>
-    <t>Exchange Act Sections 5, 15(a), and 17A(b)</t>
-  </si>
-  <si>
-    <t>Securities Act Sections 17(a)(2) and (a)(3)</t>
   </si>
   <si>
     <t>dcd-1_23-cv-02055</t>
@@ -392,36 +290,6 @@
     <t>Unjust Enrichment</t>
   </si>
   <si>
-    <t>ilnd-1_20_cv_05593</t>
-  </si>
-  <si>
-    <t>Sudhakara R. Murikinati, Jerry Nixon, Benjamin Sandmann, and Jeff S. Turnipseed</t>
-  </si>
-  <si>
-    <t>GoHealth, Inc., Clinton P. Jones, Brandon M. Cruz, Travis J. Matthiesen, NVX Holdings, Inc., Centerbridge Partners, L.P., CCP III AIV VII Holdings, L.P., CB Blizzard Co-Invest Holdings, L.P.,  Blizzard Aggregator, LLC, Centerbridge Associates III, L.P., CCP III Cayman GP Ltd., Goldman Sachs &amp; Co. LLC, BofA Securities, Inc., and Morgan Stanley &amp; Co. LLC</t>
-  </si>
-  <si>
-    <t>GOCO</t>
-  </si>
-  <si>
-    <t>nysd_1_21-cv-11222</t>
-  </si>
-  <si>
-    <t>DarkPulse, Inc.</t>
-  </si>
-  <si>
-    <t>FirstFire Global Opportunities Fund, LLC and Eli Fireman</t>
-  </si>
-  <si>
-    <t>Section 15(a) of the Act</t>
-  </si>
-  <si>
-    <t>RICO 18 U.S.C. Section 1962</t>
-  </si>
-  <si>
-    <t>Constructive Trust</t>
-  </si>
-  <si>
     <t>nysd_20_cv_04494</t>
   </si>
   <si>
@@ -500,28 +368,88 @@
     <t xml:space="preserve"> Securities Act of 1933, 15 U.S.C. Section 77e and 77l(a)(1)</t>
   </si>
   <si>
-    <t>Section 15(a) of the Exchange Act</t>
-  </si>
-  <si>
     <t>The Commodities Exchange Act, Sections 6 and 25</t>
   </si>
   <si>
     <t>Florida Securities and Investor Protection Act, Sections 517.301 and 517.211</t>
   </si>
   <si>
-    <t>Aiding and abetting violations of Exchange Act Section 10(b) and Rule 10b-5</t>
-  </si>
-  <si>
-    <t>Exchange Act Section 13(b)(2)(A)</t>
-  </si>
-  <si>
-    <t>Aiding and abetting violations of Exchange Act Section 13(b)(2)(A)</t>
-  </si>
-  <si>
-    <t>Aiding and abetting violations of Exchange Act Section 13(b)(2)(B)</t>
-  </si>
-  <si>
     <t>Civil Conspiracy</t>
+  </si>
+  <si>
+    <t>nysd_22-cv-07111</t>
+  </si>
+  <si>
+    <t>RTD Bros LLC, Todd Benn, Tom Benn, and Tomasz Rzedzian</t>
+  </si>
+  <si>
+    <t>LTRY</t>
+  </si>
+  <si>
+    <t>ctd-3-23-cv-01035</t>
+  </si>
+  <si>
+    <t>The New England Teamsters Pension Fund, Westchester Putnam Counties Heavy &amp; Highway Laborers Local 60 Benefits Fund, and United Union of Roofers, Waterproofers &amp; Allied Workers Local Union No. 8 WBPA Fund</t>
+  </si>
+  <si>
+    <t>RTX</t>
+  </si>
+  <si>
+    <t>ilnd-1-21-cv-04349</t>
+  </si>
+  <si>
+    <t>The Phoenix Insurance Company Ltd., The Phoenix Pension &amp; Provident Funds, and City of Melbourne Firefighters’ Retirement System</t>
+  </si>
+  <si>
+    <t>ATIP</t>
+  </si>
+  <si>
+    <t>ATI Physical Therapy, Inc., Labeed Diab, Joseph Jordan, Andrew A. McKnight, Joshua A. Pack, Marc Furstein, Leslee Cowen, Aaron F. Hood, Carmen A. Policy, Rakefet Russak-Aminoach, and Sunil Gulati</t>
+  </si>
+  <si>
+    <t>RTX Corporation, Gregory Hayes, Neil Mitchill, Anthony F. O’Brien, Christopher T. Calio, and Shane Eddy</t>
+  </si>
+  <si>
+    <t>Lottery.com, Inc., Lawrence Anthony “Tony” DiMatteo III, Ryan Dickinson, Matthew Clemenson, and Kathryn Lever</t>
+  </si>
+  <si>
+    <t>mad-1-21-cv-10933</t>
+  </si>
+  <si>
+    <t>mied-4-23-cv-13132</t>
+  </si>
+  <si>
+    <t>txsd-4-21-cv-02473</t>
+  </si>
+  <si>
+    <t>Julian Quinones</t>
+  </si>
+  <si>
+    <t>Frequency Therapeutics, Inc., David L. Lucchino, and Carl LeBel</t>
+  </si>
+  <si>
+    <t>FREQ</t>
+  </si>
+  <si>
+    <t>Hollywood Police Officers’ Retirement System and Plymouth County Retirement Association</t>
+  </si>
+  <si>
+    <t>General Motors Company, Cruise LLC, Mary T. Barra, Paul A. Jacobson, Kyle Vogt, Daniel Ammann, Doug L. Parks, and Wayne G. West</t>
+  </si>
+  <si>
+    <t>GM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Section 10(b) of the Exchange Act and Rule 10b-5(a)/(c) </t>
+  </si>
+  <si>
+    <t>Utah Retirement Systems and Construction Laborers Pension Trust for Southern California</t>
+  </si>
+  <si>
+    <t>CXO</t>
+  </si>
+  <si>
+    <t>Concho Resources Inc., ConocoPhillips,Timothy A. Leach, Jack F. Harper, C. William Giraud, E. Joseph Wright, and Brenda R. Schroer</t>
   </si>
 </sst>
 </file>
@@ -587,16 +515,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -901,10 +833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U29"/>
+  <dimension ref="A1:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="Q18" sqref="Q18"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H22" sqref="A22:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -952,37 +884,37 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="R1" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="S1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="T1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="3" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1035,42 +967,36 @@
         <v>34</v>
       </c>
       <c r="E3" s="2">
-        <v>44285</v>
+        <v>44515</v>
       </c>
       <c r="F3" s="2">
-        <v>44635</v>
+        <v>44776</v>
       </c>
       <c r="G3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" t="s">
-        <v>35</v>
-      </c>
-      <c r="J3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
         <v>36</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>37</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>38</v>
       </c>
-      <c r="D4" t="s">
-        <v>39</v>
-      </c>
       <c r="E4" s="2">
-        <v>44515</v>
+        <v>44621</v>
       </c>
       <c r="F4" s="2">
-        <v>44776</v>
+        <v>45372</v>
       </c>
       <c r="G4" t="s">
         <v>25</v>
@@ -1081,80 +1007,80 @@
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
         <v>40</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D5" t="s">
         <v>41</v>
       </c>
-      <c r="C5" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" t="s">
-        <v>43</v>
-      </c>
       <c r="E5" s="2">
-        <v>44621</v>
+        <v>44309</v>
       </c>
       <c r="F5" s="2">
-        <v>45372</v>
+        <v>45065</v>
       </c>
       <c r="G5" t="s">
         <v>25</v>
       </c>
       <c r="H5" t="s">
         <v>26</v>
+      </c>
+      <c r="I5" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" t="s">
         <v>44</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>45</v>
       </c>
-      <c r="C6" t="s">
-        <v>155</v>
-      </c>
-      <c r="D6" t="s">
-        <v>46</v>
-      </c>
       <c r="E6" s="2">
-        <v>44309</v>
+        <v>45245</v>
       </c>
       <c r="F6" s="2">
-        <v>45065</v>
+        <v>45511</v>
       </c>
       <c r="G6" t="s">
         <v>25</v>
       </c>
       <c r="H6" t="s">
         <v>26</v>
-      </c>
-      <c r="I6" t="s">
-        <v>28</v>
-      </c>
-      <c r="J6" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
         <v>47</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>48</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>49</v>
       </c>
-      <c r="D7" t="s">
-        <v>50</v>
-      </c>
       <c r="E7" s="2">
-        <v>45245</v>
+        <v>45132</v>
       </c>
       <c r="F7" s="2">
-        <v>45511</v>
+        <v>45223</v>
       </c>
       <c r="G7" t="s">
         <v>25</v>
@@ -1165,22 +1091,22 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
         <v>51</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>52</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>53</v>
       </c>
-      <c r="D8" t="s">
-        <v>54</v>
-      </c>
       <c r="E8" s="2">
-        <v>45132</v>
+        <v>44411</v>
       </c>
       <c r="F8" s="2">
-        <v>45223</v>
+        <v>44581</v>
       </c>
       <c r="G8" t="s">
         <v>25</v>
@@ -1191,71 +1117,74 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A9" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" t="s">
         <v>55</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" t="s">
         <v>56</v>
       </c>
-      <c r="C9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" t="s">
-        <v>58</v>
+      <c r="E9" s="2">
+        <v>43319</v>
+      </c>
+      <c r="F9" s="2">
+        <v>43329</v>
       </c>
       <c r="G9" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="H9" t="s">
-        <v>59</v>
-      </c>
-      <c r="I9" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D10" t="s">
         <v>60</v>
       </c>
-      <c r="B10" t="s">
+      <c r="E10" s="2">
+        <v>44215</v>
+      </c>
+      <c r="F10" s="2">
+        <v>44670</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" t="s">
         <v>61</v>
-      </c>
-      <c r="C10" t="s">
-        <v>62</v>
-      </c>
-      <c r="D10" t="s">
-        <v>63</v>
-      </c>
-      <c r="E10" s="2">
-        <v>44411</v>
-      </c>
-      <c r="F10" s="2">
-        <v>44581</v>
-      </c>
-      <c r="G10" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A11" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" t="s">
         <v>64</v>
       </c>
-      <c r="B11" t="s">
+      <c r="D11" t="s">
         <v>65</v>
       </c>
-      <c r="C11" t="s">
-        <v>156</v>
-      </c>
-      <c r="D11" t="s">
-        <v>66</v>
-      </c>
       <c r="E11" s="2">
-        <v>43319</v>
+        <v>44265</v>
       </c>
       <c r="F11" s="2">
-        <v>43329</v>
+        <v>45056</v>
       </c>
       <c r="G11" t="s">
         <v>25</v>
@@ -1266,54 +1195,54 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B12" t="s">
         <v>67</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>68</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>69</v>
       </c>
-      <c r="D12" t="s">
-        <v>70</v>
-      </c>
       <c r="E12" s="2">
-        <v>44215</v>
+        <v>44588</v>
       </c>
       <c r="F12" s="2">
-        <v>44670</v>
+        <v>45222</v>
       </c>
       <c r="G12" t="s">
         <v>25</v>
       </c>
       <c r="H12" t="s">
-        <v>71</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" t="s">
         <v>72</v>
       </c>
-      <c r="B13" t="s">
+      <c r="D13" t="s">
         <v>73</v>
       </c>
-      <c r="C13" t="s">
+      <c r="E13" s="2">
+        <v>44984</v>
+      </c>
+      <c r="F13" s="2">
+        <v>45169</v>
+      </c>
+      <c r="G13" t="s">
         <v>74</v>
       </c>
-      <c r="D13" t="s">
+      <c r="H13" t="s">
         <v>75</v>
-      </c>
-      <c r="E13" s="2">
-        <v>44265</v>
-      </c>
-      <c r="F13" s="2">
-        <v>45056</v>
-      </c>
-      <c r="G13" t="s">
-        <v>25</v>
-      </c>
-      <c r="H13" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.5">
@@ -1329,418 +1258,369 @@
       <c r="D14" t="s">
         <v>79</v>
       </c>
+      <c r="E14" s="2">
+        <v>42825</v>
+      </c>
+      <c r="F14" s="2">
+        <v>44187</v>
+      </c>
       <c r="G14" t="s">
-        <v>80</v>
+        <v>104</v>
       </c>
       <c r="H14" t="s">
-        <v>81</v>
-      </c>
-      <c r="I14" t="s">
-        <v>82</v>
-      </c>
-      <c r="J14" t="s">
-        <v>83</v>
-      </c>
-      <c r="K14" t="s">
-        <v>161</v>
-      </c>
-      <c r="L14" t="s">
-        <v>84</v>
-      </c>
-      <c r="M14" t="s">
-        <v>85</v>
-      </c>
-      <c r="N14" t="s">
-        <v>86</v>
-      </c>
-      <c r="O14" t="s">
-        <v>87</v>
-      </c>
-      <c r="P14" t="s">
-        <v>88</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>89</v>
-      </c>
-      <c r="R14" t="s">
-        <v>162</v>
-      </c>
-      <c r="S14" t="s">
-        <v>163</v>
-      </c>
-      <c r="T14" t="s">
-        <v>90</v>
-      </c>
-      <c r="U14" t="s">
-        <v>164</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="C15" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="G15" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="H15" t="s">
-        <v>94</v>
+        <v>25</v>
       </c>
       <c r="I15" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="J15" t="s">
-        <v>94</v>
+        <v>115</v>
       </c>
       <c r="K15" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="L15" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="M15" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="N15" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="O15" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="P15" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="Q15" t="s">
-        <v>98</v>
-      </c>
-      <c r="R15" t="s">
-        <v>98</v>
-      </c>
-      <c r="S15" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.5">
       <c r="A16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" t="s">
+        <v>91</v>
+      </c>
+      <c r="E16" s="2">
+        <v>43133</v>
+      </c>
+      <c r="F16" s="2">
+        <v>43902</v>
+      </c>
+      <c r="G16" t="s">
+        <v>25</v>
+      </c>
+      <c r="H16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A17" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" t="s">
+        <v>93</v>
+      </c>
+      <c r="C17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" t="s">
+        <v>95</v>
+      </c>
+      <c r="E17" s="2">
+        <v>44637</v>
+      </c>
+      <c r="F17" s="2">
+        <v>44826</v>
+      </c>
+      <c r="G17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A18" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D18" t="s">
+        <v>99</v>
+      </c>
+      <c r="E18" s="2">
+        <v>44505</v>
+      </c>
+      <c r="F18" s="2">
+        <v>45184</v>
+      </c>
+      <c r="G18" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A19" t="s">
         <v>100</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B19" t="s">
         <v>101</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C19" t="s">
         <v>102</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D19" t="s">
         <v>103</v>
       </c>
-      <c r="E16" s="2">
-        <v>44588</v>
-      </c>
-      <c r="F16" s="2">
-        <v>45222</v>
-      </c>
-      <c r="G16" t="s">
-        <v>25</v>
-      </c>
-      <c r="H16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.5">
-      <c r="A17" t="s">
-        <v>104</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="E19" s="2">
+        <v>44952</v>
+      </c>
+      <c r="F19" s="2">
+        <v>45505</v>
+      </c>
+      <c r="G19" t="s">
+        <v>25</v>
+      </c>
+      <c r="H19" t="s">
         <v>105</v>
       </c>
-      <c r="C17" t="s">
+      <c r="I19" t="s">
+        <v>26</v>
+      </c>
+      <c r="J19" t="s">
+        <v>28</v>
+      </c>
+      <c r="K19" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="A20" t="s">
         <v>106</v>
       </c>
-      <c r="D17" t="s">
+      <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="E17" s="2">
-        <v>44984</v>
-      </c>
-      <c r="F17" s="2">
-        <v>45169</v>
-      </c>
-      <c r="G17" t="s">
+      <c r="C20" t="s">
         <v>108</v>
       </c>
-      <c r="H17" t="s">
+      <c r="D20" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.5">
-      <c r="A18" t="s">
-        <v>110</v>
-      </c>
-      <c r="B18" t="s">
-        <v>111</v>
-      </c>
-      <c r="C18" t="s">
-        <v>112</v>
-      </c>
-      <c r="D18" t="s">
-        <v>113</v>
-      </c>
-      <c r="E18" s="2">
-        <v>42825</v>
-      </c>
-      <c r="F18" s="2">
-        <v>44187</v>
-      </c>
-      <c r="G18" t="s">
-        <v>148</v>
-      </c>
-      <c r="H18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.5">
-      <c r="A19" t="s">
-        <v>114</v>
-      </c>
-      <c r="B19" t="s">
-        <v>115</v>
-      </c>
-      <c r="C19" t="s">
-        <v>154</v>
-      </c>
-      <c r="G19" t="s">
-        <v>157</v>
-      </c>
-      <c r="H19" t="s">
-        <v>25</v>
-      </c>
-      <c r="I19" t="s">
-        <v>159</v>
-      </c>
-      <c r="J19" t="s">
-        <v>160</v>
-      </c>
-      <c r="K19" t="s">
-        <v>116</v>
-      </c>
-      <c r="L19" t="s">
+      <c r="E20" s="2">
+        <v>45127</v>
+      </c>
+      <c r="F20" s="2">
+        <v>45440</v>
+      </c>
+      <c r="G20" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A21" t="s">
         <v>117</v>
       </c>
-      <c r="M19" t="s">
+      <c r="B21" t="s">
         <v>118</v>
-      </c>
-      <c r="N19" t="s">
-        <v>119</v>
-      </c>
-      <c r="O19" t="s">
-        <v>120</v>
-      </c>
-      <c r="P19" t="s">
-        <v>121</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.5">
-      <c r="A20" t="s">
-        <v>122</v>
-      </c>
-      <c r="B20" t="s">
-        <v>123</v>
-      </c>
-      <c r="C20" t="s">
-        <v>124</v>
-      </c>
-      <c r="D20" t="s">
-        <v>125</v>
-      </c>
-      <c r="G20" t="s">
-        <v>28</v>
-      </c>
-      <c r="H20" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.5">
-      <c r="A21" t="s">
-        <v>126</v>
-      </c>
-      <c r="B21" t="s">
-        <v>127</v>
       </c>
       <c r="C21" t="s">
         <v>128</v>
       </c>
+      <c r="D21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" s="4">
+        <v>44154</v>
+      </c>
+      <c r="F21" s="4">
+        <v>44771</v>
+      </c>
       <c r="G21" t="s">
+        <v>25</v>
+      </c>
+      <c r="H21" t="s">
+        <v>26</v>
+      </c>
+      <c r="I21" t="s">
+        <v>75</v>
+      </c>
+      <c r="J21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A22" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E22" s="6">
+        <v>44235</v>
+      </c>
+      <c r="F22" s="7">
+        <v>45177</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A23" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E23" s="7">
+        <v>44249</v>
+      </c>
+      <c r="F23" s="7">
+        <v>44488</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+    </row>
+    <row r="24" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A24" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="H21" t="s">
-        <v>158</v>
-      </c>
-      <c r="I21" t="s">
-        <v>26</v>
-      </c>
-      <c r="J21" t="s">
+      <c r="B24" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="E24" s="7">
+        <v>44133</v>
+      </c>
+      <c r="F24" s="7">
+        <v>44277</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A25" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="K21" t="s">
-        <v>121</v>
-      </c>
-      <c r="L21" t="s">
+      <c r="B25" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E25" s="7">
+        <v>44251</v>
+      </c>
+      <c r="F25" s="7">
+        <v>45238</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="I25" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="5" customFormat="1" x14ac:dyDescent="0.5">
+      <c r="A26" s="5" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.5">
-      <c r="A22" t="s">
-        <v>132</v>
-      </c>
-      <c r="B22" t="s">
-        <v>133</v>
-      </c>
-      <c r="C22" t="s">
-        <v>134</v>
-      </c>
-      <c r="D22" t="s">
-        <v>135</v>
-      </c>
-      <c r="E22" s="2">
-        <v>43133</v>
-      </c>
-      <c r="F22" s="2">
-        <v>43902</v>
-      </c>
-      <c r="G22" t="s">
-        <v>25</v>
-      </c>
-      <c r="H22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.5">
-      <c r="A23" t="s">
-        <v>136</v>
-      </c>
-      <c r="B23" t="s">
-        <v>137</v>
-      </c>
-      <c r="C23" t="s">
-        <v>138</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="B26" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="E23" s="2">
-        <v>44637</v>
-      </c>
-      <c r="F23" s="2">
-        <v>44826</v>
-      </c>
-      <c r="G23" t="s">
-        <v>25</v>
-      </c>
-      <c r="H23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.5">
-      <c r="A24" t="s">
+      <c r="C26" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D26" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="B24" t="s">
-        <v>141</v>
-      </c>
-      <c r="C24" t="s">
-        <v>142</v>
-      </c>
-      <c r="D24" t="s">
-        <v>143</v>
-      </c>
-      <c r="E24" s="2">
-        <v>44505</v>
-      </c>
-      <c r="F24" s="2">
-        <v>45184</v>
-      </c>
-      <c r="G24" t="s">
-        <v>148</v>
-      </c>
-      <c r="H24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.5">
-      <c r="A25" t="s">
-        <v>144</v>
-      </c>
-      <c r="B25" t="s">
-        <v>145</v>
-      </c>
-      <c r="C25" t="s">
-        <v>146</v>
-      </c>
-      <c r="D25" t="s">
-        <v>147</v>
-      </c>
-      <c r="E25" s="2">
-        <v>44952</v>
-      </c>
-      <c r="F25" s="2">
-        <v>45505</v>
-      </c>
-      <c r="G25" t="s">
-        <v>148</v>
-      </c>
-      <c r="H25" t="s">
-        <v>149</v>
-      </c>
-      <c r="I25" t="s">
-        <v>26</v>
-      </c>
-      <c r="J25" t="s">
-        <v>28</v>
-      </c>
-      <c r="K25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.5">
-      <c r="A26" t="s">
-        <v>150</v>
-      </c>
-      <c r="B26" t="s">
-        <v>151</v>
-      </c>
-      <c r="C26" t="s">
-        <v>152</v>
-      </c>
-      <c r="D26" t="s">
-        <v>153</v>
-      </c>
-      <c r="E26" s="2">
-        <v>45127</v>
-      </c>
-      <c r="F26" s="2">
-        <v>45440</v>
-      </c>
-      <c r="G26" t="s">
-        <v>148</v>
-      </c>
-      <c r="H26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.5">
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
+      <c r="E26" s="7">
+        <v>43152</v>
+      </c>
+      <c r="F26" s="7">
+        <v>43677</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>